<commit_message>
Revise equation of errorFactor
</commit_message>
<xml_diff>
--- a/experiment_record.xlsx
+++ b/experiment_record.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="62">
   <si>
     <t>TCXO</t>
   </si>
@@ -185,6 +185,36 @@
   </si>
   <si>
     <t>2017-08-23_1304</t>
+  </si>
+  <si>
+    <t>2017-08-23_1403</t>
+  </si>
+  <si>
+    <t>2017-08-23_1405</t>
+  </si>
+  <si>
+    <t>2017-08-23_1406</t>
+  </si>
+  <si>
+    <t>2017-08-23_1434</t>
+  </si>
+  <si>
+    <t>2017-08-23_1447</t>
+  </si>
+  <si>
+    <t>2017-08-27_2056</t>
+  </si>
+  <si>
+    <t>2017-08-27_2057</t>
+  </si>
+  <si>
+    <t>2017-08-27_2058</t>
+  </si>
+  <si>
+    <t>2017-08-27_2059</t>
+  </si>
+  <si>
+    <t>2017-08-27_2100</t>
   </si>
 </sst>
 </file>
@@ -462,11 +492,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-251469584"/>
-        <c:axId val="-287573488"/>
+        <c:axId val="-1601480304"/>
+        <c:axId val="-1601477984"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-251469584"/>
+        <c:axId val="-1601480304"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -524,12 +554,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-287573488"/>
+        <c:crossAx val="-1601477984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-287573488"/>
+        <c:axId val="-1601477984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -585,7 +615,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-251469584"/>
+        <c:crossAx val="-1601480304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -793,11 +823,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-287564208"/>
-        <c:axId val="-287561888"/>
+        <c:axId val="-1636609472"/>
+        <c:axId val="-1636650720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-287564208"/>
+        <c:axId val="-1636609472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -854,12 +884,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-287561888"/>
+        <c:crossAx val="-1636650720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-287561888"/>
+        <c:axId val="-1636650720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -916,7 +946,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-287564208"/>
+        <c:crossAx val="-1636609472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2922,10 +2952,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N75"/>
+  <dimension ref="A1:N95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="O65" sqref="O65"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="A94" sqref="A94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4107,7 +4137,9 @@
       <c r="L55" s="5"/>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A57" s="5"/>
+      <c r="A57" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="B57" s="5" t="s">
         <v>28</v>
       </c>
@@ -4205,6 +4237,9 @@
       <c r="L59" s="5"/>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>53</v>
+      </c>
       <c r="B61" t="s">
         <v>38</v>
       </c>
@@ -4299,6 +4334,9 @@
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>54</v>
+      </c>
       <c r="B65" t="s">
         <v>40</v>
       </c>
@@ -4386,6 +4424,9 @@
       </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>55</v>
+      </c>
       <c r="B69" t="s">
         <v>41</v>
       </c>
@@ -4473,7 +4514,9 @@
       </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A73" s="5"/>
+      <c r="A73" s="5" t="s">
+        <v>56</v>
+      </c>
       <c r="B73" s="5" t="s">
         <v>42</v>
       </c>
@@ -4570,6 +4613,479 @@
       <c r="K75" s="5"/>
       <c r="L75" s="5"/>
     </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>57</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C77" s="6">
+        <v>1E-4</v>
+      </c>
+      <c r="D77" s="6">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="E77" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="F77" s="6">
+        <v>2E-3</v>
+      </c>
+      <c r="G77" s="6">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H77" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="I77" s="6">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="J77" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="K77" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="L77" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="M77" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="N77" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B78" s="5"/>
+      <c r="C78" s="5">
+        <v>60000</v>
+      </c>
+      <c r="D78" s="5">
+        <v>300000</v>
+      </c>
+      <c r="E78" s="5">
+        <v>600000</v>
+      </c>
+      <c r="F78" s="5">
+        <v>1800000</v>
+      </c>
+      <c r="G78" s="5">
+        <v>3600000</v>
+      </c>
+      <c r="H78" s="5">
+        <v>43200000</v>
+      </c>
+      <c r="I78" s="5">
+        <v>86400000</v>
+      </c>
+      <c r="J78" s="5"/>
+      <c r="K78" s="5"/>
+      <c r="L78" s="5"/>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B79" s="5"/>
+      <c r="C79" s="5">
+        <v>1</v>
+      </c>
+      <c r="D79" s="5">
+        <v>5</v>
+      </c>
+      <c r="E79" s="5">
+        <v>10</v>
+      </c>
+      <c r="F79" s="5">
+        <v>30</v>
+      </c>
+      <c r="G79" s="5">
+        <v>60</v>
+      </c>
+      <c r="H79" s="5">
+        <v>720</v>
+      </c>
+      <c r="I79" s="5">
+        <v>1440</v>
+      </c>
+      <c r="J79" s="5"/>
+      <c r="K79" s="5"/>
+      <c r="L79" s="5"/>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>58</v>
+      </c>
+      <c r="B81" t="s">
+        <v>38</v>
+      </c>
+      <c r="C81" s="4">
+        <v>1E-4</v>
+      </c>
+      <c r="D81" s="4">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="E81" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="F81" s="4">
+        <v>2E-3</v>
+      </c>
+      <c r="G81" s="4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H81" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="I81" s="4">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="J81" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="K81" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="L81" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="M81" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="N81" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C82">
+        <f>C83*60000</f>
+        <v>60000</v>
+      </c>
+      <c r="D82">
+        <f>D83*60000</f>
+        <v>300000</v>
+      </c>
+      <c r="E82">
+        <f t="shared" ref="E82:I82" si="11">E83*60000</f>
+        <v>600000</v>
+      </c>
+      <c r="F82">
+        <f t="shared" si="11"/>
+        <v>1800000</v>
+      </c>
+      <c r="G82">
+        <f t="shared" si="11"/>
+        <v>3600000</v>
+      </c>
+      <c r="H82">
+        <f t="shared" si="11"/>
+        <v>43200000</v>
+      </c>
+      <c r="I82">
+        <f t="shared" si="11"/>
+        <v>86400000</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C83">
+        <v>1</v>
+      </c>
+      <c r="D83">
+        <v>5</v>
+      </c>
+      <c r="E83">
+        <v>10</v>
+      </c>
+      <c r="F83">
+        <v>30</v>
+      </c>
+      <c r="G83">
+        <v>60</v>
+      </c>
+      <c r="H83">
+        <v>720</v>
+      </c>
+      <c r="I83">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>59</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C85" s="6">
+        <v>1E-4</v>
+      </c>
+      <c r="D85" s="6">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="E85" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="F85" s="6">
+        <v>2E-3</v>
+      </c>
+      <c r="G85" s="6">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H85" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="I85" s="6">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="J85" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="K85" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="L85" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="M85" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="N85" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B86" s="5"/>
+      <c r="C86" s="5">
+        <v>60000</v>
+      </c>
+      <c r="D86" s="5">
+        <v>300000</v>
+      </c>
+      <c r="E86" s="5">
+        <v>600000</v>
+      </c>
+      <c r="F86" s="5">
+        <v>1800000</v>
+      </c>
+      <c r="G86" s="5">
+        <v>3600000</v>
+      </c>
+      <c r="H86" s="5">
+        <v>43200000</v>
+      </c>
+      <c r="I86" s="5">
+        <v>86400000</v>
+      </c>
+      <c r="J86" s="5"/>
+      <c r="K86" s="5"/>
+      <c r="L86" s="5"/>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B87" s="5"/>
+      <c r="C87" s="5">
+        <v>1</v>
+      </c>
+      <c r="D87" s="5">
+        <v>5</v>
+      </c>
+      <c r="E87" s="5">
+        <v>10</v>
+      </c>
+      <c r="F87" s="5">
+        <v>30</v>
+      </c>
+      <c r="G87" s="5">
+        <v>60</v>
+      </c>
+      <c r="H87" s="5">
+        <v>720</v>
+      </c>
+      <c r="I87" s="5">
+        <v>1440</v>
+      </c>
+      <c r="J87" s="5"/>
+      <c r="K87" s="5"/>
+      <c r="L87" s="5"/>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>60</v>
+      </c>
+      <c r="B89" t="s">
+        <v>40</v>
+      </c>
+      <c r="C89" s="4">
+        <v>1E-4</v>
+      </c>
+      <c r="D89" s="4">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="E89" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="F89" s="4">
+        <v>2E-3</v>
+      </c>
+      <c r="G89" s="4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H89" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="I89" s="4">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="J89" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="K89" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="L89" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="M89" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="N89" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C90" s="5">
+        <v>60000</v>
+      </c>
+      <c r="D90" s="5">
+        <v>300000</v>
+      </c>
+      <c r="E90" s="5">
+        <v>600000</v>
+      </c>
+      <c r="F90" s="5">
+        <v>1800000</v>
+      </c>
+      <c r="G90" s="5">
+        <v>3600000</v>
+      </c>
+      <c r="H90" s="5">
+        <v>43200000</v>
+      </c>
+      <c r="I90" s="5">
+        <v>86400000</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C91" s="5">
+        <v>1</v>
+      </c>
+      <c r="D91" s="5">
+        <v>5</v>
+      </c>
+      <c r="E91" s="5">
+        <v>10</v>
+      </c>
+      <c r="F91" s="5">
+        <v>30</v>
+      </c>
+      <c r="G91" s="5">
+        <v>60</v>
+      </c>
+      <c r="H91" s="5">
+        <v>720</v>
+      </c>
+      <c r="I91" s="5">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>61</v>
+      </c>
+      <c r="B93" t="s">
+        <v>41</v>
+      </c>
+      <c r="C93" s="4">
+        <v>1E-4</v>
+      </c>
+      <c r="D93" s="4">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="E93" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="F93" s="4">
+        <v>2E-3</v>
+      </c>
+      <c r="G93" s="4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H93" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="I93" s="4">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="J93" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="K93" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="L93" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="M93" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="N93" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C94" s="5">
+        <v>60000</v>
+      </c>
+      <c r="D94" s="5">
+        <v>300000</v>
+      </c>
+      <c r="E94" s="5">
+        <v>600000</v>
+      </c>
+      <c r="F94" s="5">
+        <v>1800000</v>
+      </c>
+      <c r="G94" s="5">
+        <v>3600000</v>
+      </c>
+      <c r="H94" s="5">
+        <v>43200000</v>
+      </c>
+      <c r="I94" s="5">
+        <v>86400000</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C95" s="5">
+        <v>1</v>
+      </c>
+      <c r="D95" s="5">
+        <v>5</v>
+      </c>
+      <c r="E95" s="5">
+        <v>10</v>
+      </c>
+      <c r="F95" s="5">
+        <v>30</v>
+      </c>
+      <c r="G95" s="5">
+        <v>60</v>
+      </c>
+      <c r="H95" s="5">
+        <v>720</v>
+      </c>
+      <c r="I95" s="5">
+        <v>1440</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Revise random setting in errorFactor
</commit_message>
<xml_diff>
--- a/experiment_record.xlsx
+++ b/experiment_record.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="88">
   <si>
     <t>TCXO</t>
   </si>
@@ -215,6 +215,84 @@
   </si>
   <si>
     <t>2017-08-27_2100</t>
+  </si>
+  <si>
+    <t>time (ms)</t>
+  </si>
+  <si>
+    <t>error (ms)</t>
+  </si>
+  <si>
+    <t>revise calibration</t>
+  </si>
+  <si>
+    <t>revise errorFactor calculation</t>
+  </si>
+  <si>
+    <t>wrong run script</t>
+  </si>
+  <si>
+    <t>2017-08-27_222957</t>
+  </si>
+  <si>
+    <t>2017-08-27_223000</t>
+  </si>
+  <si>
+    <t>2017-08-27_223002</t>
+  </si>
+  <si>
+    <t>2017-08-27_223006</t>
+  </si>
+  <si>
+    <t>2017-08-27_223009</t>
+  </si>
+  <si>
+    <t>longer simTime (14day)</t>
+  </si>
+  <si>
+    <t>2017-08-28_085650</t>
+  </si>
+  <si>
+    <t>2017-08-28_091652</t>
+  </si>
+  <si>
+    <t>2017-08-28_091700</t>
+  </si>
+  <si>
+    <t>2017-08-28_091713</t>
+  </si>
+  <si>
+    <t>2017-08-28_091730</t>
+  </si>
+  <si>
+    <t>use cycle time count (1000000)</t>
+  </si>
+  <si>
+    <t>2017-08-28_132242</t>
+  </si>
+  <si>
+    <t>2017-08-28_132248</t>
+  </si>
+  <si>
+    <t>2017-08-28_132253</t>
+  </si>
+  <si>
+    <t>2017-08-28_132255</t>
+  </si>
+  <si>
+    <t>2017-08-28_155415</t>
+  </si>
+  <si>
+    <t>2017-08-28_155418</t>
+  </si>
+  <si>
+    <t>2017-08-28_155421</t>
+  </si>
+  <si>
+    <t>2017-08-28_155423</t>
+  </si>
+  <si>
+    <t>revise error factor and larger update frequency</t>
   </si>
 </sst>
 </file>
@@ -336,6 +414,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -410,6 +489,7 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -492,11 +572,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1601480304"/>
-        <c:axId val="-1601477984"/>
+        <c:axId val="941746576"/>
+        <c:axId val="941740080"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1601480304"/>
+        <c:axId val="941746576"/>
         <c:scaling>
           <c:logBase val="2.0"/>
           <c:orientation val="minMax"/>
@@ -554,12 +634,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1601477984"/>
+        <c:crossAx val="941740080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1601477984"/>
+        <c:axId val="941740080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -579,6 +659,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -615,7 +696,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1601480304"/>
+        <c:crossAx val="941746576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -679,6 +760,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -753,6 +835,7 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -823,11 +906,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1636609472"/>
-        <c:axId val="-1636650720"/>
+        <c:axId val="902217856"/>
+        <c:axId val="902309840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1636609472"/>
+        <c:axId val="902217856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -884,12 +967,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1636650720"/>
+        <c:crossAx val="902309840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1636650720"/>
+        <c:axId val="902309840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -946,7 +1029,362 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1636609472"/>
+        <c:crossAx val="902217856"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
+            <c:intercept val="0.0"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>clock_error!$H$30:$H$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.64E7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.048E8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>clock_error!$I$30:$I$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>128.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="904770464"/>
+        <c:axId val="904772944"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="904770464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="904772944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="904772944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="904770464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1075,6 +1513,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1592,6 +2070,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2211,6 +3205,36 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2479,10 +3503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView topLeftCell="F13" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36:I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2654,6 +3678,68 @@
       </c>
       <c r="C9" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="H29" t="s">
+        <v>62</v>
+      </c>
+      <c r="I29" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="H31">
+        <f>24*60*60*1000</f>
+        <v>86400000</v>
+      </c>
+      <c r="I31">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="32" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="H32">
+        <f>7*24*60*60*1000</f>
+        <v>604800000</v>
+      </c>
+      <c r="I32">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="35" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="H35">
+        <v>60000</v>
+      </c>
+      <c r="I35">
+        <f>H35*H35*0.0000000000000003+0.00000002*H35</f>
+        <v>1.2010800000000002E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="H36">
+        <f>250000-25</f>
+        <v>249975</v>
+      </c>
+      <c r="I36">
+        <f>H36*H36*0.0000000000000003+0.00000002*H36</f>
+        <v>5.0182462501875006E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="H37">
+        <v>864000000000</v>
+      </c>
+      <c r="I37">
+        <f>H37*H37*0.0000000000000003+0.00000002*H37</f>
+        <v>223966080</v>
       </c>
     </row>
   </sheetData>
@@ -2952,10 +4038,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N95"/>
+  <dimension ref="A1:N167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="A94" sqref="A94"/>
+    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="A151" sqref="A151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3553,7 +4639,9 @@
       <c r="L29" s="7"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="5"/>
+      <c r="A30" s="5" t="s">
+        <v>66</v>
+      </c>
       <c r="B30" s="5"/>
       <c r="C30" s="5">
         <v>60000</v>
@@ -3987,7 +5075,9 @@
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A50" s="5"/>
+      <c r="A50" s="5" t="s">
+        <v>66</v>
+      </c>
       <c r="B50" s="5"/>
       <c r="C50" s="5">
         <v>60000</v>
@@ -4558,7 +5648,9 @@
       </c>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A74" s="5"/>
+      <c r="A74" s="5" t="s">
+        <v>64</v>
+      </c>
       <c r="B74" s="5"/>
       <c r="C74" s="5">
         <v>60000</v>
@@ -5041,6 +6133,9 @@
       </c>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>65</v>
+      </c>
       <c r="C94" s="5">
         <v>60000</v>
       </c>
@@ -5084,6 +6179,1658 @@
       </c>
       <c r="I95" s="5">
         <v>1440</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>67</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C97" s="6">
+        <v>1E-4</v>
+      </c>
+      <c r="D97" s="6">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="E97" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="F97" s="6">
+        <v>2E-3</v>
+      </c>
+      <c r="G97" s="6">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H97" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="I97" s="6">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="J97" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="K97" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="L97" s="7">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B98" s="5"/>
+      <c r="C98" s="5">
+        <v>60000</v>
+      </c>
+      <c r="D98" s="5">
+        <v>300000</v>
+      </c>
+      <c r="E98" s="5">
+        <v>600000</v>
+      </c>
+      <c r="F98" s="5">
+        <v>1800000</v>
+      </c>
+      <c r="G98" s="5">
+        <v>3600000</v>
+      </c>
+      <c r="H98" s="5">
+        <v>43200000</v>
+      </c>
+      <c r="I98" s="5">
+        <v>86400000</v>
+      </c>
+      <c r="J98" s="5"/>
+      <c r="K98" s="5"/>
+      <c r="L98" s="5"/>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B99" s="5"/>
+      <c r="C99" s="5">
+        <v>1</v>
+      </c>
+      <c r="D99" s="5">
+        <v>5</v>
+      </c>
+      <c r="E99" s="5">
+        <v>10</v>
+      </c>
+      <c r="F99" s="5">
+        <v>30</v>
+      </c>
+      <c r="G99" s="5">
+        <v>60</v>
+      </c>
+      <c r="H99" s="5">
+        <v>720</v>
+      </c>
+      <c r="I99" s="5">
+        <v>1440</v>
+      </c>
+      <c r="J99" s="5"/>
+      <c r="K99" s="5"/>
+      <c r="L99" s="5"/>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>68</v>
+      </c>
+      <c r="B101" t="s">
+        <v>38</v>
+      </c>
+      <c r="C101" s="4">
+        <v>1E-4</v>
+      </c>
+      <c r="D101" s="4">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="E101" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="F101" s="4">
+        <v>2E-3</v>
+      </c>
+      <c r="G101" s="4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H101" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="I101" s="4">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="J101" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="K101" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="L101" s="3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C102">
+        <f>C103*60000</f>
+        <v>60000</v>
+      </c>
+      <c r="D102">
+        <f>D103*60000</f>
+        <v>300000</v>
+      </c>
+      <c r="E102">
+        <f t="shared" ref="E102:I102" si="12">E103*60000</f>
+        <v>600000</v>
+      </c>
+      <c r="F102">
+        <f t="shared" si="12"/>
+        <v>1800000</v>
+      </c>
+      <c r="G102">
+        <f t="shared" si="12"/>
+        <v>3600000</v>
+      </c>
+      <c r="H102">
+        <f t="shared" si="12"/>
+        <v>43200000</v>
+      </c>
+      <c r="I102">
+        <f t="shared" si="12"/>
+        <v>86400000</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C103">
+        <v>1</v>
+      </c>
+      <c r="D103">
+        <v>5</v>
+      </c>
+      <c r="E103">
+        <v>10</v>
+      </c>
+      <c r="F103">
+        <v>30</v>
+      </c>
+      <c r="G103">
+        <v>60</v>
+      </c>
+      <c r="H103">
+        <v>720</v>
+      </c>
+      <c r="I103">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>69</v>
+      </c>
+      <c r="B105" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C105" s="6">
+        <v>1E-4</v>
+      </c>
+      <c r="D105" s="6">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="E105" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="F105" s="6">
+        <v>2E-3</v>
+      </c>
+      <c r="G105" s="6">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H105" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="I105" s="6">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="J105" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="K105" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="L105" s="7">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B106" s="5"/>
+      <c r="C106" s="5">
+        <v>60000</v>
+      </c>
+      <c r="D106" s="5">
+        <v>300000</v>
+      </c>
+      <c r="E106" s="5">
+        <v>600000</v>
+      </c>
+      <c r="F106" s="5">
+        <v>1800000</v>
+      </c>
+      <c r="G106" s="5">
+        <v>3600000</v>
+      </c>
+      <c r="H106" s="5">
+        <v>43200000</v>
+      </c>
+      <c r="I106" s="5">
+        <v>86400000</v>
+      </c>
+      <c r="J106" s="5"/>
+      <c r="K106" s="5"/>
+      <c r="L106" s="5"/>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B107" s="5"/>
+      <c r="C107" s="5">
+        <v>1</v>
+      </c>
+      <c r="D107" s="5">
+        <v>5</v>
+      </c>
+      <c r="E107" s="5">
+        <v>10</v>
+      </c>
+      <c r="F107" s="5">
+        <v>30</v>
+      </c>
+      <c r="G107" s="5">
+        <v>60</v>
+      </c>
+      <c r="H107" s="5">
+        <v>720</v>
+      </c>
+      <c r="I107" s="5">
+        <v>1440</v>
+      </c>
+      <c r="J107" s="5"/>
+      <c r="K107" s="5"/>
+      <c r="L107" s="5"/>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>70</v>
+      </c>
+      <c r="B109" t="s">
+        <v>40</v>
+      </c>
+      <c r="C109" s="4">
+        <v>1E-4</v>
+      </c>
+      <c r="D109" s="4">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="E109" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="F109" s="4">
+        <v>2E-3</v>
+      </c>
+      <c r="G109" s="4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H109" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="I109" s="4">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="J109" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="K109" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="L109" s="3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C110" s="5">
+        <v>60000</v>
+      </c>
+      <c r="D110" s="5">
+        <v>300000</v>
+      </c>
+      <c r="E110" s="5">
+        <v>600000</v>
+      </c>
+      <c r="F110" s="5">
+        <v>1800000</v>
+      </c>
+      <c r="G110" s="5">
+        <v>3600000</v>
+      </c>
+      <c r="H110" s="5">
+        <v>43200000</v>
+      </c>
+      <c r="I110" s="5">
+        <v>86400000</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C111" s="5">
+        <v>1</v>
+      </c>
+      <c r="D111" s="5">
+        <v>5</v>
+      </c>
+      <c r="E111" s="5">
+        <v>10</v>
+      </c>
+      <c r="F111" s="5">
+        <v>30</v>
+      </c>
+      <c r="G111" s="5">
+        <v>60</v>
+      </c>
+      <c r="H111" s="5">
+        <v>720</v>
+      </c>
+      <c r="I111" s="5">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>71</v>
+      </c>
+      <c r="B113" t="s">
+        <v>41</v>
+      </c>
+      <c r="C113" s="4">
+        <v>1E-4</v>
+      </c>
+      <c r="D113" s="4">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="E113" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="F113" s="4">
+        <v>2E-3</v>
+      </c>
+      <c r="G113" s="4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H113" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="I113" s="4">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="J113" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="K113" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="L113" s="3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>72</v>
+      </c>
+      <c r="C114" s="5">
+        <v>60000</v>
+      </c>
+      <c r="D114" s="5">
+        <v>300000</v>
+      </c>
+      <c r="E114" s="5">
+        <v>600000</v>
+      </c>
+      <c r="F114" s="5">
+        <v>1800000</v>
+      </c>
+      <c r="G114" s="5">
+        <v>3600000</v>
+      </c>
+      <c r="H114" s="5">
+        <v>43200000</v>
+      </c>
+      <c r="I114" s="5">
+        <v>86400000</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C115" s="5">
+        <v>1</v>
+      </c>
+      <c r="D115" s="5">
+        <v>5</v>
+      </c>
+      <c r="E115" s="5">
+        <v>10</v>
+      </c>
+      <c r="F115" s="5">
+        <v>30</v>
+      </c>
+      <c r="G115" s="5">
+        <v>60</v>
+      </c>
+      <c r="H115" s="5">
+        <v>720</v>
+      </c>
+      <c r="I115" s="5">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>73</v>
+      </c>
+      <c r="B117" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C117" s="6">
+        <v>1E-4</v>
+      </c>
+      <c r="D117" s="6">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="E117" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="F117" s="6">
+        <v>2E-3</v>
+      </c>
+      <c r="G117" s="6">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H117" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="I117" s="6">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="J117" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="K117" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="L117" s="7">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B118" s="5"/>
+      <c r="C118" s="5">
+        <v>60000</v>
+      </c>
+      <c r="D118" s="5">
+        <v>300000</v>
+      </c>
+      <c r="E118" s="5">
+        <v>600000</v>
+      </c>
+      <c r="F118" s="5">
+        <v>1800000</v>
+      </c>
+      <c r="G118" s="5">
+        <v>3600000</v>
+      </c>
+      <c r="H118" s="5">
+        <v>43200000</v>
+      </c>
+      <c r="I118" s="5">
+        <v>86400000</v>
+      </c>
+      <c r="J118" s="5"/>
+      <c r="K118" s="5"/>
+      <c r="L118" s="5"/>
+    </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B119" s="5"/>
+      <c r="C119" s="5">
+        <v>1</v>
+      </c>
+      <c r="D119" s="5">
+        <v>5</v>
+      </c>
+      <c r="E119" s="5">
+        <v>10</v>
+      </c>
+      <c r="F119" s="5">
+        <v>30</v>
+      </c>
+      <c r="G119" s="5">
+        <v>60</v>
+      </c>
+      <c r="H119" s="5">
+        <v>720</v>
+      </c>
+      <c r="I119" s="5">
+        <v>1440</v>
+      </c>
+      <c r="J119" s="5"/>
+      <c r="K119" s="5"/>
+      <c r="L119" s="5"/>
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>74</v>
+      </c>
+      <c r="B121" t="s">
+        <v>38</v>
+      </c>
+      <c r="C121" s="4">
+        <v>1E-4</v>
+      </c>
+      <c r="D121" s="4">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="E121" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="F121" s="4">
+        <v>2E-3</v>
+      </c>
+      <c r="G121" s="4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H121" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="I121" s="4">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="J121" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="K121" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="L121" s="3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C122">
+        <f>C123*60000</f>
+        <v>60000</v>
+      </c>
+      <c r="D122">
+        <f>D123*60000</f>
+        <v>300000</v>
+      </c>
+      <c r="E122">
+        <f t="shared" ref="E122:I122" si="13">E123*60000</f>
+        <v>600000</v>
+      </c>
+      <c r="F122">
+        <f t="shared" si="13"/>
+        <v>1800000</v>
+      </c>
+      <c r="G122">
+        <f t="shared" si="13"/>
+        <v>3600000</v>
+      </c>
+      <c r="H122">
+        <f t="shared" si="13"/>
+        <v>43200000</v>
+      </c>
+      <c r="I122">
+        <f t="shared" si="13"/>
+        <v>86400000</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C123">
+        <v>1</v>
+      </c>
+      <c r="D123">
+        <v>5</v>
+      </c>
+      <c r="E123">
+        <v>10</v>
+      </c>
+      <c r="F123">
+        <v>30</v>
+      </c>
+      <c r="G123">
+        <v>60</v>
+      </c>
+      <c r="H123">
+        <v>720</v>
+      </c>
+      <c r="I123">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>75</v>
+      </c>
+      <c r="B125" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C125" s="6">
+        <v>1E-4</v>
+      </c>
+      <c r="D125" s="6">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="E125" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="F125" s="6">
+        <v>2E-3</v>
+      </c>
+      <c r="G125" s="6">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H125" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="I125" s="6">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="J125" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="K125" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="L125" s="7">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B126" s="5"/>
+      <c r="C126" s="5">
+        <v>60000</v>
+      </c>
+      <c r="D126" s="5">
+        <v>300000</v>
+      </c>
+      <c r="E126" s="5">
+        <v>600000</v>
+      </c>
+      <c r="F126" s="5">
+        <v>1800000</v>
+      </c>
+      <c r="G126" s="5">
+        <v>3600000</v>
+      </c>
+      <c r="H126" s="5">
+        <v>43200000</v>
+      </c>
+      <c r="I126" s="5">
+        <v>86400000</v>
+      </c>
+      <c r="J126" s="5"/>
+      <c r="K126" s="5"/>
+      <c r="L126" s="5"/>
+    </row>
+    <row r="127" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B127" s="5"/>
+      <c r="C127" s="5">
+        <v>1</v>
+      </c>
+      <c r="D127" s="5">
+        <v>5</v>
+      </c>
+      <c r="E127" s="5">
+        <v>10</v>
+      </c>
+      <c r="F127" s="5">
+        <v>30</v>
+      </c>
+      <c r="G127" s="5">
+        <v>60</v>
+      </c>
+      <c r="H127" s="5">
+        <v>720</v>
+      </c>
+      <c r="I127" s="5">
+        <v>1440</v>
+      </c>
+      <c r="J127" s="5"/>
+      <c r="K127" s="5"/>
+      <c r="L127" s="5"/>
+    </row>
+    <row r="129" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>76</v>
+      </c>
+      <c r="B129" t="s">
+        <v>40</v>
+      </c>
+      <c r="C129" s="4">
+        <v>1E-4</v>
+      </c>
+      <c r="D129" s="4">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="E129" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="F129" s="4">
+        <v>2E-3</v>
+      </c>
+      <c r="G129" s="4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H129" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="I129" s="4">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="J129" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="K129" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="L129" s="3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C130" s="5">
+        <v>60000</v>
+      </c>
+      <c r="D130" s="5">
+        <v>300000</v>
+      </c>
+      <c r="E130" s="5">
+        <v>600000</v>
+      </c>
+      <c r="F130" s="5">
+        <v>1800000</v>
+      </c>
+      <c r="G130" s="5">
+        <v>3600000</v>
+      </c>
+      <c r="H130" s="5">
+        <v>43200000</v>
+      </c>
+      <c r="I130" s="5">
+        <v>86400000</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C131" s="5">
+        <v>1</v>
+      </c>
+      <c r="D131" s="5">
+        <v>5</v>
+      </c>
+      <c r="E131" s="5">
+        <v>10</v>
+      </c>
+      <c r="F131" s="5">
+        <v>30</v>
+      </c>
+      <c r="G131" s="5">
+        <v>60</v>
+      </c>
+      <c r="H131" s="5">
+        <v>720</v>
+      </c>
+      <c r="I131" s="5">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>77</v>
+      </c>
+      <c r="B133" t="s">
+        <v>41</v>
+      </c>
+      <c r="C133" s="4">
+        <v>1E-4</v>
+      </c>
+      <c r="D133" s="4">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="E133" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="F133" s="4">
+        <v>2E-3</v>
+      </c>
+      <c r="G133" s="4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H133" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="I133" s="4">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="J133" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="K133" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="L133" s="3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>78</v>
+      </c>
+      <c r="C134" s="5">
+        <v>60000</v>
+      </c>
+      <c r="D134" s="5">
+        <v>300000</v>
+      </c>
+      <c r="E134" s="5">
+        <v>600000</v>
+      </c>
+      <c r="F134" s="5">
+        <v>1800000</v>
+      </c>
+      <c r="G134" s="5">
+        <v>3600000</v>
+      </c>
+      <c r="H134" s="5">
+        <v>43200000</v>
+      </c>
+      <c r="I134" s="5">
+        <v>86400000</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C135" s="5">
+        <v>1</v>
+      </c>
+      <c r="D135" s="5">
+        <v>5</v>
+      </c>
+      <c r="E135" s="5">
+        <v>10</v>
+      </c>
+      <c r="F135" s="5">
+        <v>30</v>
+      </c>
+      <c r="G135" s="5">
+        <v>60</v>
+      </c>
+      <c r="H135" s="5">
+        <v>720</v>
+      </c>
+      <c r="I135" s="5">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="137" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>79</v>
+      </c>
+      <c r="B137" t="s">
+        <v>38</v>
+      </c>
+      <c r="C137" s="4">
+        <v>1E-4</v>
+      </c>
+      <c r="D137" s="4">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="E137" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="F137" s="4">
+        <v>2E-3</v>
+      </c>
+      <c r="G137" s="4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H137" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="I137" s="4">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="J137" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="K137" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="L137" s="3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C138">
+        <f>C139*60000</f>
+        <v>60000</v>
+      </c>
+      <c r="D138">
+        <f>D139*60000</f>
+        <v>300000</v>
+      </c>
+      <c r="E138">
+        <f t="shared" ref="E138:I138" si="14">E139*60000</f>
+        <v>600000</v>
+      </c>
+      <c r="F138">
+        <f t="shared" si="14"/>
+        <v>1800000</v>
+      </c>
+      <c r="G138">
+        <f t="shared" si="14"/>
+        <v>3600000</v>
+      </c>
+      <c r="H138">
+        <f t="shared" si="14"/>
+        <v>43200000</v>
+      </c>
+      <c r="I138">
+        <f t="shared" si="14"/>
+        <v>86400000</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C139">
+        <v>1</v>
+      </c>
+      <c r="D139">
+        <v>5</v>
+      </c>
+      <c r="E139">
+        <v>10</v>
+      </c>
+      <c r="F139">
+        <v>30</v>
+      </c>
+      <c r="G139">
+        <v>60</v>
+      </c>
+      <c r="H139">
+        <v>720</v>
+      </c>
+      <c r="I139">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="141" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>80</v>
+      </c>
+      <c r="B141" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C141" s="6">
+        <v>1E-4</v>
+      </c>
+      <c r="D141" s="6">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="E141" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="F141" s="6">
+        <v>2E-3</v>
+      </c>
+      <c r="G141" s="6">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H141" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="I141" s="6">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="J141" s="7">
+        <v>0.05</v>
+      </c>
+      <c r="K141" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="L141" s="7">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="142" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B142" s="5"/>
+      <c r="C142" s="5">
+        <v>60000</v>
+      </c>
+      <c r="D142" s="5">
+        <v>300000</v>
+      </c>
+      <c r="E142" s="5">
+        <v>600000</v>
+      </c>
+      <c r="F142" s="5">
+        <v>1800000</v>
+      </c>
+      <c r="G142" s="5">
+        <v>3600000</v>
+      </c>
+      <c r="H142" s="5">
+        <v>43200000</v>
+      </c>
+      <c r="I142" s="5">
+        <v>86400000</v>
+      </c>
+      <c r="J142" s="5"/>
+      <c r="K142" s="5"/>
+      <c r="L142" s="5"/>
+    </row>
+    <row r="143" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B143" s="5"/>
+      <c r="C143" s="5">
+        <v>1</v>
+      </c>
+      <c r="D143" s="5">
+        <v>5</v>
+      </c>
+      <c r="E143" s="5">
+        <v>10</v>
+      </c>
+      <c r="F143" s="5">
+        <v>30</v>
+      </c>
+      <c r="G143" s="5">
+        <v>60</v>
+      </c>
+      <c r="H143" s="5">
+        <v>720</v>
+      </c>
+      <c r="I143" s="5">
+        <v>1440</v>
+      </c>
+      <c r="J143" s="5"/>
+      <c r="K143" s="5"/>
+      <c r="L143" s="5"/>
+    </row>
+    <row r="145" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>81</v>
+      </c>
+      <c r="B145" t="s">
+        <v>40</v>
+      </c>
+      <c r="C145" s="4">
+        <v>1E-4</v>
+      </c>
+      <c r="D145" s="4">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="E145" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="F145" s="4">
+        <v>2E-3</v>
+      </c>
+      <c r="G145" s="4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H145" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="I145" s="4">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="J145" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="K145" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="L145" s="3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="146" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C146" s="5">
+        <v>60000</v>
+      </c>
+      <c r="D146" s="5">
+        <v>300000</v>
+      </c>
+      <c r="E146" s="5">
+        <v>600000</v>
+      </c>
+      <c r="F146" s="5">
+        <v>1800000</v>
+      </c>
+      <c r="G146" s="5">
+        <v>3600000</v>
+      </c>
+      <c r="H146" s="5">
+        <v>43200000</v>
+      </c>
+      <c r="I146" s="5">
+        <v>86400000</v>
+      </c>
+    </row>
+    <row r="147" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C147" s="5">
+        <v>1</v>
+      </c>
+      <c r="D147" s="5">
+        <v>5</v>
+      </c>
+      <c r="E147" s="5">
+        <v>10</v>
+      </c>
+      <c r="F147" s="5">
+        <v>30</v>
+      </c>
+      <c r="G147" s="5">
+        <v>60</v>
+      </c>
+      <c r="H147" s="5">
+        <v>720</v>
+      </c>
+      <c r="I147" s="5">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="149" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>82</v>
+      </c>
+      <c r="B149" t="s">
+        <v>41</v>
+      </c>
+      <c r="C149" s="4">
+        <v>1E-4</v>
+      </c>
+      <c r="D149" s="4">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="E149" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="F149" s="4">
+        <v>2E-3</v>
+      </c>
+      <c r="G149" s="4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H149" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="I149" s="4">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="J149" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="K149" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="L149" s="3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>87</v>
+      </c>
+      <c r="C150" s="5">
+        <v>60000</v>
+      </c>
+      <c r="D150" s="5">
+        <v>300000</v>
+      </c>
+      <c r="E150" s="5">
+        <v>600000</v>
+      </c>
+      <c r="F150" s="5">
+        <v>1800000</v>
+      </c>
+      <c r="G150" s="5">
+        <v>3600000</v>
+      </c>
+      <c r="H150" s="5">
+        <v>43200000</v>
+      </c>
+      <c r="I150" s="5">
+        <v>86400000</v>
+      </c>
+    </row>
+    <row r="151" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C151" s="5">
+        <v>1</v>
+      </c>
+      <c r="D151" s="5">
+        <v>5</v>
+      </c>
+      <c r="E151" s="5">
+        <v>10</v>
+      </c>
+      <c r="F151" s="5">
+        <v>30</v>
+      </c>
+      <c r="G151" s="5">
+        <v>60</v>
+      </c>
+      <c r="H151" s="5">
+        <v>720</v>
+      </c>
+      <c r="I151" s="5">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="153" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>83</v>
+      </c>
+      <c r="B153" t="s">
+        <v>38</v>
+      </c>
+      <c r="C153" s="4">
+        <v>1E-4</v>
+      </c>
+      <c r="D153" s="4">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="E153" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="F153" s="4">
+        <v>2E-3</v>
+      </c>
+      <c r="G153" s="4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H153" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="I153" s="4">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="J153" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="K153" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="L153" s="3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="154" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C154">
+        <f>C155*60000</f>
+        <v>60000</v>
+      </c>
+      <c r="D154">
+        <f>D155*60000</f>
+        <v>3600000</v>
+      </c>
+      <c r="E154">
+        <f>E155*60000</f>
+        <v>43200000</v>
+      </c>
+      <c r="F154">
+        <f>F155*60000</f>
+        <v>86400000</v>
+      </c>
+      <c r="G154">
+        <f>G155*60000</f>
+        <v>172800000</v>
+      </c>
+      <c r="H154">
+        <f>H155*60000</f>
+        <v>345600000</v>
+      </c>
+      <c r="I154">
+        <f>I155*60000</f>
+        <v>691200000</v>
+      </c>
+      <c r="J154">
+        <f>J155*60000</f>
+        <v>864000000</v>
+      </c>
+    </row>
+    <row r="155" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C155">
+        <v>1</v>
+      </c>
+      <c r="D155">
+        <v>60</v>
+      </c>
+      <c r="E155">
+        <v>720</v>
+      </c>
+      <c r="F155">
+        <v>1440</v>
+      </c>
+      <c r="G155">
+        <v>2880</v>
+      </c>
+      <c r="H155">
+        <f>G155*2</f>
+        <v>5760</v>
+      </c>
+      <c r="I155">
+        <f>H155*2</f>
+        <v>11520</v>
+      </c>
+      <c r="J155">
+        <f>F155*10</f>
+        <v>14400</v>
+      </c>
+    </row>
+    <row r="157" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>84</v>
+      </c>
+      <c r="B157" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C157" s="4">
+        <v>1E-4</v>
+      </c>
+      <c r="D157" s="4">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="E157" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="F157" s="4">
+        <v>2E-3</v>
+      </c>
+      <c r="G157" s="4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H157" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="I157" s="4">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="J157" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="K157" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="L157" s="3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="158" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B158" s="5"/>
+      <c r="C158">
+        <f>C159*60000</f>
+        <v>60000</v>
+      </c>
+      <c r="D158">
+        <f>D159*60000</f>
+        <v>3600000</v>
+      </c>
+      <c r="E158">
+        <f>E159*60000</f>
+        <v>43200000</v>
+      </c>
+      <c r="F158">
+        <f>F159*60000</f>
+        <v>86400000</v>
+      </c>
+      <c r="G158">
+        <f>G159*60000</f>
+        <v>172800000</v>
+      </c>
+      <c r="H158">
+        <f>H159*60000</f>
+        <v>345600000</v>
+      </c>
+      <c r="I158">
+        <f>I159*60000</f>
+        <v>691200000</v>
+      </c>
+      <c r="J158">
+        <f>J159*60000</f>
+        <v>864000000</v>
+      </c>
+    </row>
+    <row r="159" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B159" s="5"/>
+      <c r="C159">
+        <v>1</v>
+      </c>
+      <c r="D159">
+        <v>60</v>
+      </c>
+      <c r="E159">
+        <v>720</v>
+      </c>
+      <c r="F159">
+        <v>1440</v>
+      </c>
+      <c r="G159">
+        <v>2880</v>
+      </c>
+      <c r="H159">
+        <f>G159*2</f>
+        <v>5760</v>
+      </c>
+      <c r="I159">
+        <f>H159*2</f>
+        <v>11520</v>
+      </c>
+      <c r="J159">
+        <f>F159*10</f>
+        <v>14400</v>
+      </c>
+    </row>
+    <row r="161" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>85</v>
+      </c>
+      <c r="B161" t="s">
+        <v>40</v>
+      </c>
+      <c r="C161" s="4">
+        <v>1E-4</v>
+      </c>
+      <c r="D161" s="4">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="E161" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="F161" s="4">
+        <v>2E-3</v>
+      </c>
+      <c r="G161" s="4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H161" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="I161" s="4">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="J161" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="K161" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="L161" s="3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="162" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C162">
+        <f>C163*60000</f>
+        <v>60000</v>
+      </c>
+      <c r="D162">
+        <f>D163*60000</f>
+        <v>3600000</v>
+      </c>
+      <c r="E162">
+        <f>E163*60000</f>
+        <v>43200000</v>
+      </c>
+      <c r="F162">
+        <f>F163*60000</f>
+        <v>86400000</v>
+      </c>
+      <c r="G162">
+        <f>G163*60000</f>
+        <v>172800000</v>
+      </c>
+      <c r="H162">
+        <f>H163*60000</f>
+        <v>345600000</v>
+      </c>
+      <c r="I162">
+        <f>I163*60000</f>
+        <v>691200000</v>
+      </c>
+      <c r="J162">
+        <f>J163*60000</f>
+        <v>864000000</v>
+      </c>
+    </row>
+    <row r="163" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C163">
+        <v>1</v>
+      </c>
+      <c r="D163">
+        <v>60</v>
+      </c>
+      <c r="E163">
+        <v>720</v>
+      </c>
+      <c r="F163">
+        <v>1440</v>
+      </c>
+      <c r="G163">
+        <v>2880</v>
+      </c>
+      <c r="H163">
+        <f>G163*2</f>
+        <v>5760</v>
+      </c>
+      <c r="I163">
+        <f>H163*2</f>
+        <v>11520</v>
+      </c>
+      <c r="J163">
+        <f>F163*10</f>
+        <v>14400</v>
+      </c>
+    </row>
+    <row r="165" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>86</v>
+      </c>
+      <c r="B165" t="s">
+        <v>41</v>
+      </c>
+      <c r="C165" s="4">
+        <v>1E-4</v>
+      </c>
+      <c r="D165" s="4">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="E165" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="F165" s="4">
+        <v>2E-3</v>
+      </c>
+      <c r="G165" s="4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H165" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="I165" s="4">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="J165" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="K165" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="L165" s="3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="166" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C166">
+        <f>C167*60000</f>
+        <v>60000</v>
+      </c>
+      <c r="D166">
+        <f>D167*60000</f>
+        <v>3600000</v>
+      </c>
+      <c r="E166">
+        <f>E167*60000</f>
+        <v>43200000</v>
+      </c>
+      <c r="F166">
+        <f>F167*60000</f>
+        <v>86400000</v>
+      </c>
+      <c r="G166">
+        <f>G167*60000</f>
+        <v>172800000</v>
+      </c>
+      <c r="H166">
+        <f>H167*60000</f>
+        <v>345600000</v>
+      </c>
+      <c r="I166">
+        <f>I167*60000</f>
+        <v>691200000</v>
+      </c>
+      <c r="J166">
+        <f>J167*60000</f>
+        <v>864000000</v>
+      </c>
+    </row>
+    <row r="167" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C167">
+        <v>1</v>
+      </c>
+      <c r="D167">
+        <v>60</v>
+      </c>
+      <c r="E167">
+        <v>720</v>
+      </c>
+      <c r="F167">
+        <v>1440</v>
+      </c>
+      <c r="G167">
+        <v>2880</v>
+      </c>
+      <c r="H167">
+        <f>G167*2</f>
+        <v>5760</v>
+      </c>
+      <c r="I167">
+        <f>H167*2</f>
+        <v>11520</v>
+      </c>
+      <c r="J167">
+        <f>F167*10</f>
+        <v>14400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>